<commit_message>
correção de datas no template
</commit_message>
<xml_diff>
--- a/docs/template_csll.xlsx
+++ b/docs/template_csll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_projects\dev\superveniencia_csll\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A4918F-D2E5-4E41-8FE6-1CF706A3ABBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C074AE5E-FA51-4233-9CB9-ECB6F812295C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{284B33CC-1D1C-45F5-8082-6FFD49238665}"/>
   </bookViews>
@@ -378,7 +378,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="88">
     <dxf>
       <font>
         <b/>
@@ -391,6 +391,105 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -534,9 +633,6 @@
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -545,6 +641,9 @@
       <font>
         <b/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -749,17 +848,17 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight3">
     <tableStyle name="PivotStyleLight3 2" table="0" count="11" xr9:uid="{D4C6F8C2-21AC-43C8-A44F-EFC1566C1FFB}">
-      <tableStyleElement type="wholeTable" dxfId="64"/>
-      <tableStyleElement type="headerRow" dxfId="63"/>
-      <tableStyleElement type="totalRow" dxfId="62"/>
-      <tableStyleElement type="firstRowStripe" dxfId="61"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="60"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="59"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="58"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="57"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="56"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="55"/>
-      <tableStyleElement type="pageFieldValues" dxfId="54"/>
+      <tableStyleElement type="wholeTable" dxfId="87"/>
+      <tableStyleElement type="headerRow" dxfId="86"/>
+      <tableStyleElement type="totalRow" dxfId="85"/>
+      <tableStyleElement type="firstRowStripe" dxfId="84"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="83"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="82"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="81"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="80"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="79"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="78"/>
+      <tableStyleElement type="pageFieldValues" dxfId="77"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -9348,10 +9447,648 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9F902641-16D6-4B87-8B06-ABEF29C750DB}" name="PivotTable14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B275:D278" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="18"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="17">
+        <item m="1" x="15"/>
+        <item h="1" x="4"/>
+        <item x="12"/>
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Movimentacao" fld="7" baseField="1" baseItem="13" numFmtId="43"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E193453-EA67-48A9-8342-81AFE67F49F6}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B160:M181" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="18"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="17">
+        <item m="1" x="15"/>
+        <item h="1" x="4"/>
+        <item h="1" x="12"/>
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="20">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Movimentacao" fld="7" baseField="1" baseItem="10" numFmtId="43"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A27AAB2C-A37C-4D78-8BC0-9781BC059C37}" name="PivotTable21" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B314:M316" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="17">
+        <item h="1" x="10"/>
+        <item h="1" x="8"/>
+        <item m="1" x="15"/>
+        <item h="1" x="4"/>
+        <item h="1" x="12"/>
+        <item h="1" x="3"/>
+        <item h="1" x="6"/>
+        <item m="1" x="13"/>
+        <item x="11"/>
+        <item m="1" x="14"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="5"/>
+        <item h="1" x="9"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="1"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item m="1" x="9"/>
+        <item m="1" x="10"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="5" numFmtId="43"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="64">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="63">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="61">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight3 2" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3DD79EEC-BC91-46BB-B3AC-A19E947AC627}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B82:M84" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="17">
+        <item m="1" x="15"/>
+        <item h="1" x="4"/>
+        <item h="1" x="12"/>
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item x="3"/>
+        <item m="1" x="10"/>
+        <item m="1" x="9"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Movimentacao" fld="7" baseField="0" baseItem="0" numFmtId="43"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="67">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="66">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="65">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8BAA3150-16F3-430D-8468-864E05A2F7D6}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B20:M41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
       <items count="12">
         <item x="0"/>
         <item x="1"/>
@@ -9551,11 +10288,11 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2293AFA-67CC-4D49-807A-8AE400C85707}" name="PivotTable17" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B238:M240" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2F3F7F63-09E5-433D-9BFE-F40EDFC08F4D}" name="PivotTable18" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B141:M143" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
       <items count="12">
         <item x="0"/>
         <item x="1"/>
@@ -9576,7 +10313,7 @@
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="17">
         <item h="1" x="10"/>
-        <item h="1" x="8"/>
+        <item x="8"/>
         <item m="1" x="15"/>
         <item h="1" x="4"/>
         <item h="1" x="12"/>
@@ -9589,7 +10326,7 @@
         <item h="1" x="2"/>
         <item h="1" x="0"/>
         <item h="1" x="5"/>
-        <item x="9"/>
+        <item h="1" x="9"/>
         <item h="1" x="7"/>
         <item t="default"/>
       </items>
@@ -9620,7 +10357,7 @@
   </rowFields>
   <rowItems count="1">
     <i>
-      <x v="7"/>
+      <x v="2"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -9665,31 +10402,22 @@
     <pageField fld="3" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="7" numFmtId="43"/>
+    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="2" numFmtId="43"/>
   </dataFields>
-  <formats count="4">
-    <format dxfId="34">
+  <formats count="3">
+    <format dxfId="70">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
-            <x v="8"/>
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="32">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="31">
+    <format dxfId="68">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -9711,11 +10439,11 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A27AAB2C-A37C-4D78-8BC0-9781BC059C37}" name="PivotTable21" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B314:M316" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E4F28BB-603F-45D2-86E1-CA71F38B3967}" name="PivotTable12" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B251:M254" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
       <items count="12">
         <item x="0"/>
         <item x="1"/>
@@ -9731,56 +10459,78 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="18"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="17">
-        <item h="1" x="10"/>
-        <item h="1" x="8"/>
         <item m="1" x="15"/>
-        <item h="1" x="4"/>
+        <item x="4"/>
         <item h="1" x="12"/>
-        <item h="1" x="3"/>
-        <item h="1" x="6"/>
         <item m="1" x="13"/>
-        <item x="11"/>
         <item m="1" x="14"/>
         <item h="1" x="1"/>
         <item h="1" x="2"/>
         <item h="1" x="0"/>
+        <item h="1" x="3"/>
         <item h="1" x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
         <item h="1" x="9"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item x="1"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item m="1" x="9"/>
-        <item m="1" x="10"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item m="1" x="11"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
   </rowFields>
-  <rowItems count="1">
+  <rowItems count="2">
     <i>
-      <x v="5"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -9817,55 +10567,17 @@
     <i>
       <x v="9"/>
     </i>
-    <i>
-      <x v="10"/>
+    <i t="grand">
+      <x/>
     </i>
   </colItems>
   <pageFields count="1">
     <pageField fld="3" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="5" numFmtId="43"/>
+    <dataField name="Sum of Movimentacao" fld="7" baseField="2" baseItem="3" numFmtId="43"/>
   </dataFields>
-  <formats count="4">
-    <format dxfId="38">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="37">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="36">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="35">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight3 2" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -9877,11 +10589,162 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D92BBDF3-86B3-4630-BA5D-8E4B12DF8619}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B246:M248" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="17">
+        <item m="1" x="15"/>
+        <item x="4"/>
+        <item h="1" x="12"/>
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item x="3"/>
+        <item m="1" x="10"/>
+        <item m="1" x="9"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="0" numFmtId="43"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="73">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="72">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="71">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BCCE0F1C-DB7E-4097-91EE-6CEC1DBBD817}" name="PivotTable8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B114:M117" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
       <items count="12">
         <item x="0"/>
         <item x="1"/>
@@ -10027,11 +10890,162 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2EB8C729-20E4-41E8-9E42-A4435106DD30}" name="PivotTable19" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B299:M301" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="17">
+        <item x="10"/>
+        <item h="1" x="8"/>
+        <item m="1" x="15"/>
+        <item h="1" x="4"/>
+        <item h="1" x="12"/>
+        <item h="1" x="3"/>
+        <item h="1" x="6"/>
+        <item m="1" x="13"/>
+        <item h="1" x="11"/>
+        <item m="1" x="14"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="5"/>
+        <item h="1" x="9"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="1"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item m="1" x="9"/>
+        <item m="1" x="10"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="1" numFmtId="43"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="41">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="40">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="39">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight3 2" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8593AC4E-B6FD-4FDD-812A-736707F1F5F7}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B87:M90" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
       <items count="12">
         <item x="0"/>
         <item x="1"/>
@@ -10177,11 +11191,162 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{762768C0-31CC-4B0D-BE8D-75A75D63B7C8}" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B152:M154" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="17">
+        <item m="1" x="15"/>
+        <item h="1" x="4"/>
+        <item h="1" x="12"/>
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item x="3"/>
+        <item m="1" x="10"/>
+        <item m="1" x="9"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="4" numFmtId="43"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="44">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="43">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="42">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A3A3FDB7-7E76-4332-9464-121C68FE3F16}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Total Geral" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B9:M11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
       <items count="12">
         <item x="0"/>
         <item x="1"/>
@@ -10294,10 +11459,10 @@
     <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="2" numFmtId="43"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="41">
+    <format dxfId="47">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -10306,7 +11471,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="45">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -10328,11 +11493,446 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9880B853-8AB8-4A4F-AE2D-5AFBDF03617D}" name="PivotTable13" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B270:D272" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="17">
+        <item m="1" x="15"/>
+        <item h="1" x="4"/>
+        <item x="12"/>
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item x="3"/>
+        <item m="1" x="10"/>
+        <item m="1" x="9"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="1" numFmtId="43"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="50">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="49">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="48">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{02769CB7-F854-445D-8D83-265823CD9293}" name="PivotTable15" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B76:M78" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="17">
+        <item m="1" x="15"/>
+        <item h="1" x="4"/>
+        <item h="1" x="12"/>
+        <item h="1" x="3"/>
+        <item h="1" x="6"/>
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="5"/>
+        <item x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="1"/>
+        <item m="1" x="9"/>
+        <item m="1" x="10"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x v="7"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="7" numFmtId="43"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="53">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="52">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="51">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight3 2" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2293AFA-67CC-4D49-807A-8AE400C85707}" name="PivotTable17" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B238:M240" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="12">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="17">
+        <item h="1" x="10"/>
+        <item h="1" x="8"/>
+        <item m="1" x="15"/>
+        <item h="1" x="4"/>
+        <item h="1" x="12"/>
+        <item h="1" x="3"/>
+        <item h="1" x="6"/>
+        <item m="1" x="13"/>
+        <item h="1" x="11"/>
+        <item m="1" x="14"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="5"/>
+        <item x="9"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="1"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item m="1" x="9"/>
+        <item m="1" x="10"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x v="7"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="7" numFmtId="43"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="57">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="56">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="55">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="54">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight3 2" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{295CA191-B576-42F0-B6CB-AB26C1B7B963}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B108:M110" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
       <items count="12">
         <item x="0"/>
         <item x="1"/>
@@ -10445,10 +12045,10 @@
     <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="1" numFmtId="43"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="44">
+    <format dxfId="60">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="59">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -10457,1508 +12057,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2F3F7F63-09E5-433D-9BFE-F40EDFC08F4D}" name="PivotTable18" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B141:M143" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
-        <item h="1" x="10"/>
-        <item x="8"/>
-        <item m="1" x="15"/>
-        <item h="1" x="4"/>
-        <item h="1" x="12"/>
-        <item h="1" x="3"/>
-        <item h="1" x="6"/>
-        <item m="1" x="13"/>
-        <item h="1" x="11"/>
-        <item m="1" x="14"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item h="1" x="5"/>
-        <item h="1" x="9"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item x="1"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item m="1" x="9"/>
-        <item m="1" x="10"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="1">
-    <i>
-      <x v="2"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="2" numFmtId="43"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="47">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="46">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="45">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight3 2" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D92BBDF3-86B3-4630-BA5D-8E4B12DF8619}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B246:M248" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
-        <item m="1" x="15"/>
-        <item x="4"/>
-        <item h="1" x="12"/>
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item x="3"/>
-        <item m="1" x="10"/>
-        <item m="1" x="9"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="1">
-    <i>
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="0" numFmtId="43"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="50">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="49">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="48">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E4F28BB-603F-45D2-86E1-CA71F38B3967}" name="PivotTable12" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B251:M254" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="19"/>
-        <item x="18"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
-        <item m="1" x="15"/>
-        <item x="4"/>
-        <item h="1" x="12"/>
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="2" baseItem="3" numFmtId="43"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2EB8C729-20E4-41E8-9E42-A4435106DD30}" name="PivotTable19" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B299:M301" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
-        <item x="10"/>
-        <item h="1" x="8"/>
-        <item m="1" x="15"/>
-        <item h="1" x="4"/>
-        <item h="1" x="12"/>
-        <item h="1" x="3"/>
-        <item h="1" x="6"/>
-        <item m="1" x="13"/>
-        <item h="1" x="11"/>
-        <item m="1" x="14"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item h="1" x="5"/>
-        <item h="1" x="9"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item x="1"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item m="1" x="9"/>
-        <item m="1" x="10"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="1">
-    <i>
-      <x v="1"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="1" numFmtId="43"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="18">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="17">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="16">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight3 2" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{02769CB7-F854-445D-8D83-265823CD9293}" name="PivotTable15" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B76:M78" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
-        <item m="1" x="15"/>
-        <item h="1" x="4"/>
-        <item h="1" x="12"/>
-        <item h="1" x="3"/>
-        <item h="1" x="6"/>
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item h="1" x="5"/>
-        <item x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item x="1"/>
-        <item m="1" x="9"/>
-        <item m="1" x="10"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="1">
-    <i>
-      <x v="7"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="7" numFmtId="43"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="21">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="20">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="19">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight3 2" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E193453-EA67-48A9-8342-81AFE67F49F6}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B160:M181" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="19"/>
-        <item x="18"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
-        <item m="1" x="15"/>
-        <item h="1" x="4"/>
-        <item h="1" x="12"/>
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="20">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="1" baseItem="10" numFmtId="43"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3DD79EEC-BC91-46BB-B3AC-A19E947AC627}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B82:M84" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
-        <item m="1" x="15"/>
-        <item h="1" x="4"/>
-        <item h="1" x="12"/>
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item x="3"/>
-        <item m="1" x="10"/>
-        <item m="1" x="9"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="1">
-    <i>
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="0" baseItem="0" numFmtId="43"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="24">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="23">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="22">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9F902641-16D6-4B87-8B06-ABEF29C750DB}" name="PivotTable14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B275:D278" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="22">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="19"/>
-        <item x="18"/>
-        <item x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
-        <item m="1" x="15"/>
-        <item h="1" x="4"/>
-        <item x="12"/>
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="1" baseItem="13" numFmtId="43"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{762768C0-31CC-4B0D-BE8D-75A75D63B7C8}" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B152:M154" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
-        <item m="1" x="15"/>
-        <item h="1" x="4"/>
-        <item h="1" x="12"/>
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item x="3"/>
-        <item m="1" x="10"/>
-        <item m="1" x="9"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="1">
-    <i>
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="4" numFmtId="43"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="27">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="26">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9880B853-8AB8-4A4F-AE2D-5AFBDF03617D}" name="PivotTable13" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B270:D272" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="8">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="17">
-        <item m="1" x="15"/>
-        <item h="1" x="4"/>
-        <item x="12"/>
-        <item m="1" x="13"/>
-        <item m="1" x="14"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item x="3"/>
-        <item m="1" x="10"/>
-        <item m="1" x="9"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="1">
-    <i>
-      <x v="1"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Movimentacao" fld="7" baseField="4" baseItem="1" numFmtId="43"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="30">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="29">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="28">
+    <format dxfId="58">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -11987,10 +12086,10 @@
     <tableColumn id="1" xr3:uid="{4352CCD2-E1AE-4F7F-83B1-8BDFF3316472}" name="Ano"/>
     <tableColumn id="2" xr3:uid="{91F1E4F1-AD20-43A9-8D1A-3B7BFD50CA97}" name="Conta_Nome"/>
     <tableColumn id="3" xr3:uid="{9FFF1985-B721-44A0-8B14-346B01ED5700}" name="Cosif_Nome"/>
-    <tableColumn id="4" xr3:uid="{311A7484-C75A-472D-89C7-CB9BB8F63958}" name="Tributo" dataDxfId="53" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{68D6235F-94FF-480C-85F5-6B337BCCE1E3}" name="Descrição" dataDxfId="52" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{311A7484-C75A-472D-89C7-CB9BB8F63958}" name="Tributo" dataDxfId="76" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{68D6235F-94FF-480C-85F5-6B337BCCE1E3}" name="Descrição" dataDxfId="75" dataCellStyle="Comma"/>
     <tableColumn id="6" xr3:uid="{59363A9F-5B0B-46BE-9B58-172FB506062D}" name="ValorDebito"/>
-    <tableColumn id="7" xr3:uid="{7B2C1D67-F616-4CA1-8207-7DD605A91F7D}" name="ValorCredito" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{7B2C1D67-F616-4CA1-8207-7DD605A91F7D}" name="ValorCredito" dataDxfId="74"/>
     <tableColumn id="8" xr3:uid="{493C8851-65FC-4F0B-B9D5-DD20920D9B2A}" name="Movimentacao"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -33759,8 +33858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72FB3FD-D0E7-492E-9DB5-519453722DB1}">
   <dimension ref="A1:N333"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A277" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B316" sqref="B316"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>